<commit_message>
add trafo data in excel
</commit_message>
<xml_diff>
--- a/stability_analysis/data/cases/IEEE_118_FULL_headers.xlsx
+++ b/stability_analysis/data/cases/IEEE_118_FULL_headers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20404"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Francesca\Documents\stability_analysis\stability_analysis\data\cases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Francesca\Documents\StabilityAnalysis\stability_analysis\data\cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD8B6087-08ED-4401-B1B3-4A5022CE2364}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D561F4-B02B-499E-8D19-BA7CA790DFBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="1455" windowWidth="28800" windowHeight="17505" tabRatio="922" firstSheet="2" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="922" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gen" sheetId="20" r:id="rId1"/>
@@ -30,6 +30,17 @@
     <sheet name="sim" sheetId="17" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -861,9 +872,9 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" s="20" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A1" s="33" t="s">
         <v>23</v>
       </c>
@@ -917,9 +928,9 @@
       <selection activeCell="M2" sqref="M2:M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>23</v>
       </c>
@@ -960,7 +971,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -975,7 +986,7 @@
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -990,7 +1001,7 @@
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -1018,21 +1029,21 @@
       <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="5.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="5.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="6.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="2"/>
+    <col min="10" max="10" width="4.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -1091,7 +1102,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="K8" s="15"/>
     </row>
   </sheetData>
@@ -1108,12 +1119,12 @@
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="33" t="s">
         <v>23</v>
       </c>
@@ -1154,7 +1165,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="30"/>
       <c r="B2" s="30"/>
       <c r="C2" s="30"/>
@@ -1167,7 +1178,7 @@
       <c r="J2" s="30"/>
       <c r="K2" s="30"/>
     </row>
-    <row r="3" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="30"/>
       <c r="B3" s="30"/>
       <c r="C3" s="30"/>
@@ -1179,7 +1190,7 @@
       <c r="I3" s="30"/>
       <c r="J3" s="30"/>
     </row>
-    <row r="4" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="30"/>
       <c r="B4" s="30"/>
       <c r="C4" s="30"/>
@@ -1191,7 +1202,7 @@
       <c r="I4" s="30"/>
       <c r="J4" s="30"/>
     </row>
-    <row r="5" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="30"/>
       <c r="B5" s="30"/>
       <c r="C5" s="30"/>
@@ -1203,7 +1214,7 @@
       <c r="I5" s="30"/>
       <c r="J5" s="30"/>
     </row>
-    <row r="6" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="30"/>
       <c r="B6" s="30"/>
       <c r="C6" s="30"/>
@@ -1215,7 +1226,7 @@
       <c r="I6" s="30"/>
       <c r="J6" s="30"/>
     </row>
-    <row r="7" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="30"/>
       <c r="B7" s="30"/>
       <c r="C7" s="30"/>
@@ -1227,56 +1238,56 @@
       <c r="I7" s="30"/>
       <c r="J7" s="30"/>
     </row>
-    <row r="8" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="K11" s="37"/>
       <c r="L11" s="37"/>
       <c r="M11" s="37"/>
       <c r="N11" s="37"/>
     </row>
-    <row r="12" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="K12" s="37"/>
       <c r="L12" s="37"/>
       <c r="M12" s="37"/>
       <c r="N12" s="37"/>
     </row>
-    <row r="13" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="K13" s="37"/>
       <c r="L13" s="37"/>
       <c r="M13" s="37"/>
       <c r="N13" s="37"/>
     </row>
-    <row r="14" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="17" s="32" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="18" s="32" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="19" s="32" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="20" s="32" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="21" s="32" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="22" s="32" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="23" s="32" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="24" s="32" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="25" s="32" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" s="32" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" s="32" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" s="32" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" s="32" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" s="32" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" s="32" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" s="32" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="32" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="32" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="32" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="32" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="32" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="32" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="32" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="32" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="32" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="32" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="17" s="32" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="18" s="32" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="19" s="32" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="20" s="32" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="21" s="32" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="22" s="32" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="23" s="32" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="24" s="32" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="25" s="32" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="26" s="32" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="27" s="32" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="28" s="32" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="29" s="32" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="30" s="32" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="31" s="32" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="32" s="32" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="33" s="32" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="34" s="32" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="35" s="32" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="36" s="32" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="37" s="32" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="38" s="32" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="39" s="32" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="40" s="32" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="41" s="32" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="42" s="32" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1291,12 +1302,12 @@
       <selection activeCell="A2" sqref="A2:XFD115"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="8.7109375" style="4"/>
+    <col min="1" max="16384" width="8.6640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="34" t="s">
         <v>46</v>
       </c>
@@ -1310,679 +1321,679 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2"/>
       <c r="B2"/>
       <c r="C2"/>
       <c r="D2"/>
     </row>
-    <row r="3" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3"/>
       <c r="B3"/>
       <c r="C3"/>
       <c r="D3"/>
     </row>
-    <row r="4" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4"/>
       <c r="B4"/>
       <c r="C4"/>
       <c r="D4"/>
     </row>
-    <row r="5" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5"/>
       <c r="B5"/>
       <c r="C5"/>
       <c r="D5"/>
     </row>
-    <row r="6" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6"/>
       <c r="B6"/>
       <c r="C6"/>
       <c r="D6"/>
     </row>
-    <row r="7" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7"/>
       <c r="B7"/>
       <c r="C7"/>
       <c r="D7"/>
     </row>
-    <row r="8" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8"/>
       <c r="B8"/>
       <c r="C8"/>
       <c r="D8"/>
     </row>
-    <row r="9" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9"/>
       <c r="B9"/>
       <c r="C9"/>
       <c r="D9"/>
     </row>
-    <row r="10" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10"/>
       <c r="B10"/>
       <c r="C10"/>
       <c r="D10"/>
     </row>
-    <row r="11" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11"/>
       <c r="B11"/>
       <c r="C11"/>
       <c r="D11"/>
     </row>
-    <row r="12" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12"/>
       <c r="B12"/>
       <c r="C12"/>
       <c r="D12"/>
     </row>
-    <row r="13" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13"/>
       <c r="B13"/>
       <c r="C13"/>
       <c r="D13"/>
     </row>
-    <row r="14" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14"/>
       <c r="B14"/>
       <c r="C14"/>
       <c r="D14"/>
     </row>
-    <row r="15" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15"/>
       <c r="B15"/>
       <c r="C15"/>
       <c r="D15"/>
     </row>
-    <row r="16" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16"/>
       <c r="B16"/>
       <c r="C16"/>
       <c r="D16"/>
     </row>
-    <row r="17" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17"/>
       <c r="B17"/>
       <c r="C17"/>
       <c r="D17"/>
     </row>
-    <row r="18" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18"/>
       <c r="B18"/>
       <c r="C18"/>
       <c r="D18"/>
     </row>
-    <row r="19" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19"/>
       <c r="B19"/>
       <c r="C19"/>
       <c r="D19"/>
     </row>
-    <row r="20" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20"/>
       <c r="B20"/>
       <c r="C20"/>
       <c r="D20"/>
     </row>
-    <row r="21" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21"/>
       <c r="B21"/>
       <c r="C21"/>
       <c r="D21"/>
     </row>
-    <row r="22" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22"/>
       <c r="B22"/>
       <c r="C22"/>
       <c r="D22"/>
     </row>
-    <row r="23" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23"/>
       <c r="B23"/>
       <c r="C23"/>
       <c r="D23"/>
     </row>
-    <row r="24" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24"/>
       <c r="B24"/>
       <c r="C24"/>
       <c r="D24"/>
     </row>
-    <row r="25" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25"/>
       <c r="B25"/>
       <c r="C25"/>
       <c r="D25"/>
     </row>
-    <row r="26" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26"/>
       <c r="B26"/>
       <c r="C26"/>
       <c r="D26"/>
     </row>
-    <row r="27" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27"/>
       <c r="B27"/>
       <c r="C27"/>
       <c r="D27"/>
     </row>
-    <row r="28" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28"/>
       <c r="B28"/>
       <c r="C28"/>
       <c r="D28"/>
     </row>
-    <row r="29" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29"/>
       <c r="B29"/>
       <c r="C29"/>
       <c r="D29"/>
     </row>
-    <row r="30" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30"/>
       <c r="B30"/>
       <c r="C30"/>
       <c r="D30"/>
     </row>
-    <row r="31" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31"/>
       <c r="B31"/>
       <c r="C31"/>
       <c r="D31"/>
     </row>
-    <row r="32" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32"/>
       <c r="B32"/>
       <c r="C32"/>
       <c r="D32"/>
     </row>
-    <row r="33" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33"/>
       <c r="B33"/>
       <c r="C33"/>
       <c r="D33"/>
     </row>
-    <row r="34" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34"/>
       <c r="B34"/>
       <c r="C34"/>
       <c r="D34"/>
     </row>
-    <row r="35" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35"/>
       <c r="B35"/>
       <c r="C35"/>
       <c r="D35"/>
     </row>
-    <row r="36" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36"/>
       <c r="B36"/>
       <c r="C36"/>
       <c r="D36"/>
     </row>
-    <row r="37" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37"/>
       <c r="B37"/>
       <c r="C37"/>
       <c r="D37"/>
     </row>
-    <row r="38" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38"/>
       <c r="B38"/>
       <c r="C38"/>
       <c r="D38"/>
     </row>
-    <row r="39" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39"/>
       <c r="B39"/>
       <c r="C39"/>
       <c r="D39"/>
     </row>
-    <row r="40" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40"/>
       <c r="B40"/>
       <c r="C40"/>
       <c r="D40"/>
     </row>
-    <row r="41" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41"/>
       <c r="B41"/>
       <c r="C41"/>
       <c r="D41"/>
     </row>
-    <row r="42" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42"/>
       <c r="B42"/>
       <c r="C42"/>
       <c r="D42"/>
     </row>
-    <row r="43" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43"/>
       <c r="B43"/>
       <c r="C43"/>
       <c r="D43"/>
     </row>
-    <row r="44" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44"/>
       <c r="B44"/>
       <c r="C44"/>
       <c r="D44"/>
     </row>
-    <row r="45" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45"/>
       <c r="B45"/>
       <c r="C45"/>
       <c r="D45"/>
     </row>
-    <row r="46" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46"/>
       <c r="B46"/>
       <c r="C46"/>
       <c r="D46"/>
     </row>
-    <row r="47" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47"/>
       <c r="B47"/>
       <c r="C47"/>
       <c r="D47"/>
     </row>
-    <row r="48" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48"/>
       <c r="B48"/>
       <c r="C48"/>
       <c r="D48"/>
     </row>
-    <row r="49" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49"/>
       <c r="B49"/>
       <c r="C49"/>
       <c r="D49"/>
     </row>
-    <row r="50" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50"/>
       <c r="B50"/>
       <c r="C50"/>
       <c r="D50"/>
     </row>
-    <row r="51" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51"/>
       <c r="B51"/>
       <c r="C51"/>
       <c r="D51"/>
     </row>
-    <row r="52" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52"/>
       <c r="B52"/>
       <c r="C52"/>
       <c r="D52"/>
     </row>
-    <row r="53" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53"/>
       <c r="B53"/>
       <c r="C53"/>
       <c r="D53"/>
     </row>
-    <row r="54" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54"/>
       <c r="B54"/>
       <c r="C54"/>
       <c r="D54"/>
     </row>
-    <row r="55" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55"/>
       <c r="B55"/>
       <c r="C55"/>
       <c r="D55"/>
     </row>
-    <row r="56" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56"/>
       <c r="B56"/>
       <c r="C56"/>
       <c r="D56"/>
     </row>
-    <row r="57" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57"/>
       <c r="B57"/>
       <c r="C57"/>
       <c r="D57"/>
     </row>
-    <row r="58" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58"/>
       <c r="B58"/>
       <c r="C58"/>
       <c r="D58"/>
     </row>
-    <row r="59" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59"/>
       <c r="B59"/>
       <c r="C59"/>
       <c r="D59"/>
     </row>
-    <row r="60" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60"/>
       <c r="B60"/>
       <c r="C60"/>
       <c r="D60"/>
     </row>
-    <row r="61" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61"/>
       <c r="B61"/>
       <c r="C61"/>
       <c r="D61"/>
     </row>
-    <row r="62" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62"/>
       <c r="B62"/>
       <c r="C62"/>
       <c r="D62"/>
     </row>
-    <row r="63" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63"/>
       <c r="B63"/>
       <c r="C63"/>
       <c r="D63"/>
     </row>
-    <row r="64" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64"/>
       <c r="B64"/>
       <c r="C64"/>
       <c r="D64"/>
     </row>
-    <row r="65" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65"/>
       <c r="B65"/>
       <c r="C65"/>
       <c r="D65"/>
     </row>
-    <row r="66" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A66"/>
       <c r="B66"/>
       <c r="C66"/>
       <c r="D66"/>
     </row>
-    <row r="67" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A67"/>
       <c r="B67"/>
       <c r="C67"/>
       <c r="D67"/>
     </row>
-    <row r="68" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A68"/>
       <c r="B68"/>
       <c r="C68"/>
       <c r="D68"/>
     </row>
-    <row r="69" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69"/>
       <c r="B69"/>
       <c r="C69"/>
       <c r="D69"/>
     </row>
-    <row r="70" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A70"/>
       <c r="B70"/>
       <c r="C70"/>
       <c r="D70"/>
     </row>
-    <row r="71" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A71"/>
       <c r="B71"/>
       <c r="C71"/>
       <c r="D71"/>
     </row>
-    <row r="72" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A72"/>
       <c r="B72"/>
       <c r="C72"/>
       <c r="D72"/>
     </row>
-    <row r="73" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A73"/>
       <c r="B73"/>
       <c r="C73"/>
       <c r="D73"/>
     </row>
-    <row r="74" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A74"/>
       <c r="B74"/>
       <c r="C74"/>
       <c r="D74"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75"/>
       <c r="B75"/>
       <c r="C75"/>
       <c r="D75"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76"/>
       <c r="B76"/>
       <c r="C76"/>
       <c r="D76"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77"/>
       <c r="B77"/>
       <c r="C77"/>
       <c r="D77"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78"/>
       <c r="B78"/>
       <c r="C78"/>
       <c r="D78"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79"/>
       <c r="B79"/>
       <c r="C79"/>
       <c r="D79"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80"/>
       <c r="B80"/>
       <c r="C80"/>
       <c r="D80"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81"/>
       <c r="B81"/>
       <c r="C81"/>
       <c r="D81"/>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82"/>
       <c r="B82"/>
       <c r="C82"/>
       <c r="D82"/>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83"/>
       <c r="B83"/>
       <c r="C83"/>
       <c r="D83"/>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84"/>
       <c r="B84"/>
       <c r="C84"/>
       <c r="D84"/>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85"/>
       <c r="B85"/>
       <c r="C85"/>
       <c r="D85"/>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86"/>
       <c r="B86"/>
       <c r="C86"/>
       <c r="D86"/>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87"/>
       <c r="B87"/>
       <c r="C87"/>
       <c r="D87"/>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88"/>
       <c r="B88"/>
       <c r="C88"/>
       <c r="D88"/>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89"/>
       <c r="B89"/>
       <c r="C89"/>
       <c r="D89"/>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90"/>
       <c r="B90"/>
       <c r="C90"/>
       <c r="D90"/>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91"/>
       <c r="B91"/>
       <c r="C91"/>
       <c r="D91"/>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92"/>
       <c r="B92"/>
       <c r="C92"/>
       <c r="D92"/>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93"/>
       <c r="B93"/>
       <c r="C93"/>
       <c r="D93"/>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94"/>
       <c r="B94"/>
       <c r="C94"/>
       <c r="D94"/>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95"/>
       <c r="B95"/>
       <c r="C95"/>
       <c r="D95"/>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96"/>
       <c r="B96"/>
       <c r="C96"/>
       <c r="D96"/>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97"/>
       <c r="B97"/>
       <c r="C97"/>
       <c r="D97"/>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98"/>
       <c r="B98"/>
       <c r="C98"/>
       <c r="D98"/>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99"/>
       <c r="B99"/>
       <c r="C99"/>
       <c r="D99"/>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100"/>
       <c r="B100"/>
       <c r="C100"/>
       <c r="D100"/>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101"/>
       <c r="B101"/>
       <c r="C101"/>
       <c r="D101"/>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102"/>
       <c r="B102"/>
       <c r="C102"/>
       <c r="D102"/>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103"/>
       <c r="B103"/>
       <c r="C103"/>
       <c r="D103"/>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104"/>
       <c r="B104"/>
       <c r="C104"/>
       <c r="D104"/>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105"/>
       <c r="B105"/>
       <c r="C105"/>
       <c r="D105"/>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106"/>
       <c r="B106"/>
       <c r="C106"/>
       <c r="D106"/>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107"/>
       <c r="B107"/>
       <c r="C107"/>
       <c r="D107"/>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108"/>
       <c r="B108"/>
       <c r="C108"/>
       <c r="D108"/>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109"/>
       <c r="B109"/>
       <c r="C109"/>
       <c r="D109"/>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110"/>
       <c r="B110"/>
       <c r="C110"/>
       <c r="D110"/>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111"/>
       <c r="B111"/>
       <c r="C111"/>
       <c r="D111"/>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112"/>
       <c r="B112"/>
       <c r="C112"/>
       <c r="D112"/>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113"/>
       <c r="B113"/>
       <c r="C113"/>
       <c r="D113"/>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114"/>
       <c r="B114"/>
       <c r="C114"/>
@@ -2001,14 +2012,14 @@
       <selection activeCell="A2" sqref="A2:XFD34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="1"/>
-    <col min="3" max="4" width="9.140625" style="52"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="2" width="9.109375" style="1"/>
+    <col min="3" max="4" width="9.109375" style="52"/>
+    <col min="5" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
@@ -2028,62 +2039,62 @@
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="43"/>
       <c r="C2" s="47"/>
       <c r="D2" s="47"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="43"/>
       <c r="C3" s="47"/>
       <c r="D3" s="47"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="43"/>
       <c r="C4" s="47"/>
       <c r="D4" s="47"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="43"/>
       <c r="C5" s="47"/>
       <c r="D5" s="47"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="43"/>
       <c r="C6" s="47"/>
       <c r="D6" s="47"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="43"/>
       <c r="C7" s="47"/>
       <c r="D7" s="47"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="43"/>
       <c r="C8" s="47"/>
       <c r="D8" s="47"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="43"/>
       <c r="C9" s="47"/>
       <c r="D9" s="47"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="43"/>
       <c r="C10" s="47"/>
       <c r="D10" s="47"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="43"/>
       <c r="C11" s="47"/>
       <c r="D11" s="47"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="43"/>
       <c r="C12" s="47"/>
       <c r="D12" s="47"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="48"/>
       <c r="B13" s="49"/>
       <c r="C13" s="50"/>
@@ -2091,82 +2102,82 @@
       <c r="E13" s="49"/>
       <c r="F13" s="49"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="43"/>
       <c r="C14" s="47"/>
       <c r="D14" s="47"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="43"/>
       <c r="C15" s="47"/>
       <c r="D15" s="47"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="43"/>
       <c r="C16" s="47"/>
       <c r="D16" s="47"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="43"/>
       <c r="C17" s="47"/>
       <c r="D17" s="47"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="43"/>
       <c r="C18" s="47"/>
       <c r="D18" s="47"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="43"/>
       <c r="C19" s="47"/>
       <c r="D19" s="47"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="43"/>
       <c r="C20" s="47"/>
       <c r="D20" s="47"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="43"/>
       <c r="C21" s="47"/>
       <c r="D21" s="47"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="43"/>
       <c r="C22" s="47"/>
       <c r="D22" s="47"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="43"/>
       <c r="C23" s="47"/>
       <c r="D23" s="47"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="43"/>
       <c r="C24" s="47"/>
       <c r="D24" s="47"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="43"/>
       <c r="C25" s="47"/>
       <c r="D25" s="47"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="43"/>
       <c r="C26" s="47"/>
       <c r="D26" s="47"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="43"/>
       <c r="C27" s="47"/>
       <c r="D27" s="47"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="43"/>
       <c r="C28" s="47"/>
       <c r="D28" s="47"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="43"/>
       <c r="C29" s="47"/>
       <c r="D29" s="47"/>
@@ -2180,16 +2191,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CE4402C-C892-4185-ACFC-0918E41EF0CD}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="33" t="s">
         <v>50</v>
       </c>
@@ -2212,7 +2223,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="38"/>
       <c r="B2" s="38"/>
       <c r="C2" s="37"/>
@@ -2231,14 +2242,14 @@
       <selection activeCell="F4" sqref="A2:F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="8.7109375" style="7"/>
-    <col min="6" max="6" width="10.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.7109375" style="7"/>
+    <col min="1" max="5" width="8.6640625" style="7"/>
+    <col min="6" max="6" width="10.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.6640625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>57</v>
       </c>
@@ -2258,11 +2269,11 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E2" s="8"/>
     </row>
-    <row r="5" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777778" bottom="1.0527777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2281,12 +2292,12 @@
       <selection activeCell="A2" sqref="A2:H168"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="33" t="s">
         <v>23</v>
       </c>
@@ -2309,121 +2320,121 @@
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F28" s="3"/>
     </row>
   </sheetData>
@@ -2444,12 +2455,12 @@
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="8.7109375" style="8"/>
+    <col min="1" max="16384" width="8.6640625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>23</v>
       </c>
@@ -2496,19 +2507,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E717AAA3-63C1-47BF-9E0D-1A781E3C2FDE}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="8.7109375" style="11"/>
-    <col min="7" max="7" width="10.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" style="11"/>
-    <col min="9" max="16384" width="8.7109375" style="13"/>
+    <col min="1" max="6" width="8.6640625" style="11"/>
+    <col min="7" max="7" width="10.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" style="11"/>
+    <col min="9" max="16384" width="8.6640625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="28" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>23</v>
       </c>
@@ -2537,44 +2548,274 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="F2" s="12"/>
-      <c r="I2"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="F3" s="12"/>
-      <c r="I3"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="E4" s="41"/>
-      <c r="F4" s="12"/>
-      <c r="I4"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D5" s="12"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="12"/>
-      <c r="I5"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D6" s="12"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="12"/>
-      <c r="I6"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="F7" s="12"/>
-      <c r="I7"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="F8" s="12"/>
-      <c r="I8"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I9"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I10"/>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="11">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11">
+        <v>5</v>
+      </c>
+      <c r="C2" s="11">
+        <v>8</v>
+      </c>
+      <c r="D2" s="11">
+        <v>0</v>
+      </c>
+      <c r="E2" s="11">
+        <v>1E-4</v>
+      </c>
+      <c r="F2" s="12">
+        <v>0</v>
+      </c>
+      <c r="G2" s="11">
+        <v>1</v>
+      </c>
+      <c r="H2" s="11">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="11">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="11">
+        <v>17</v>
+      </c>
+      <c r="C3" s="11">
+        <v>30</v>
+      </c>
+      <c r="D3" s="11">
+        <v>0</v>
+      </c>
+      <c r="E3" s="11">
+        <v>1E-4</v>
+      </c>
+      <c r="F3" s="12">
+        <v>0</v>
+      </c>
+      <c r="G3" s="11">
+        <v>1</v>
+      </c>
+      <c r="H3" s="11">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="11">
+        <f t="shared" ref="A4:A10" si="0">A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="11">
+        <v>25</v>
+      </c>
+      <c r="C4" s="11">
+        <v>26</v>
+      </c>
+      <c r="D4" s="11">
+        <v>0</v>
+      </c>
+      <c r="E4" s="41">
+        <v>1E-4</v>
+      </c>
+      <c r="F4" s="12">
+        <v>0</v>
+      </c>
+      <c r="G4" s="11">
+        <v>1</v>
+      </c>
+      <c r="H4" s="11">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="11">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B5" s="11">
+        <v>37</v>
+      </c>
+      <c r="C5" s="11">
+        <v>38</v>
+      </c>
+      <c r="D5" s="12">
+        <v>0</v>
+      </c>
+      <c r="E5" s="41">
+        <v>1E-4</v>
+      </c>
+      <c r="F5" s="12">
+        <v>0</v>
+      </c>
+      <c r="G5" s="11">
+        <v>1</v>
+      </c>
+      <c r="H5" s="11">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="11">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="11">
+        <v>59</v>
+      </c>
+      <c r="C6" s="11">
+        <v>63</v>
+      </c>
+      <c r="D6" s="12">
+        <v>0</v>
+      </c>
+      <c r="E6" s="41">
+        <v>1E-4</v>
+      </c>
+      <c r="F6" s="12">
+        <v>0</v>
+      </c>
+      <c r="G6" s="11">
+        <v>1</v>
+      </c>
+      <c r="H6" s="11">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="11">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="11">
+        <v>61</v>
+      </c>
+      <c r="C7" s="11">
+        <v>64</v>
+      </c>
+      <c r="D7" s="11">
+        <v>0</v>
+      </c>
+      <c r="E7" s="11">
+        <v>1E-4</v>
+      </c>
+      <c r="F7" s="12">
+        <v>0</v>
+      </c>
+      <c r="G7" s="11">
+        <v>1</v>
+      </c>
+      <c r="H7" s="11">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="11">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="11">
+        <v>65</v>
+      </c>
+      <c r="C8" s="11">
+        <v>66</v>
+      </c>
+      <c r="D8" s="11">
+        <v>0</v>
+      </c>
+      <c r="E8" s="11">
+        <v>1E-4</v>
+      </c>
+      <c r="F8" s="12">
+        <v>0</v>
+      </c>
+      <c r="G8" s="11">
+        <v>1</v>
+      </c>
+      <c r="H8" s="11">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="11">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="11">
+        <v>68</v>
+      </c>
+      <c r="C9" s="11">
+        <v>69</v>
+      </c>
+      <c r="D9" s="11">
+        <v>0</v>
+      </c>
+      <c r="E9" s="11">
+        <v>1E-4</v>
+      </c>
+      <c r="F9" s="11">
+        <v>0</v>
+      </c>
+      <c r="G9" s="11">
+        <v>1</v>
+      </c>
+      <c r="H9" s="11">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="11">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="11">
+        <v>80</v>
+      </c>
+      <c r="C10" s="11">
+        <v>81</v>
+      </c>
+      <c r="D10" s="11">
+        <v>0</v>
+      </c>
+      <c r="E10" s="11">
+        <v>1E-4</v>
+      </c>
+      <c r="F10" s="11">
+        <v>0</v>
+      </c>
+      <c r="G10" s="11">
+        <v>1</v>
+      </c>
+      <c r="H10" s="11">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2589,14 +2830,14 @@
       <selection activeCell="A2" sqref="A2:I92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="6" width="8.7109375" style="2"/>
-    <col min="7" max="7" width="8.7109375" style="10"/>
-    <col min="8" max="16384" width="8.7109375" style="2"/>
+    <col min="1" max="6" width="8.6640625" style="2"/>
+    <col min="7" max="7" width="8.6640625" style="10"/>
+    <col min="8" max="16384" width="8.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="33" t="s">
         <v>23</v>
       </c>
@@ -2622,7 +2863,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B2"/>
       <c r="E2"/>
       <c r="F2"/>
@@ -2630,7 +2871,7 @@
       <c r="J2"/>
       <c r="K2"/>
     </row>
-    <row r="3" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B3"/>
       <c r="E3"/>
       <c r="F3"/>
@@ -2638,7 +2879,7 @@
       <c r="J3"/>
       <c r="K3"/>
     </row>
-    <row r="4" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B4"/>
       <c r="E4"/>
       <c r="F4"/>
@@ -2646,7 +2887,7 @@
       <c r="J4"/>
       <c r="K4"/>
     </row>
-    <row r="5" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B5"/>
       <c r="E5"/>
       <c r="F5"/>
@@ -2654,7 +2895,7 @@
       <c r="J5"/>
       <c r="K5"/>
     </row>
-    <row r="6" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B6"/>
       <c r="E6"/>
       <c r="F6"/>
@@ -2662,7 +2903,7 @@
       <c r="J6"/>
       <c r="K6"/>
     </row>
-    <row r="7" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B7"/>
       <c r="E7"/>
       <c r="F7"/>
@@ -2670,7 +2911,7 @@
       <c r="J7"/>
       <c r="K7"/>
     </row>
-    <row r="8" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B8"/>
       <c r="E8"/>
       <c r="F8"/>
@@ -2678,7 +2919,7 @@
       <c r="J8"/>
       <c r="K8"/>
     </row>
-    <row r="9" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B9"/>
       <c r="E9"/>
       <c r="F9"/>
@@ -2686,7 +2927,7 @@
       <c r="J9"/>
       <c r="K9"/>
     </row>
-    <row r="10" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B10"/>
       <c r="E10"/>
       <c r="F10"/>
@@ -2694,7 +2935,7 @@
       <c r="J10"/>
       <c r="K10"/>
     </row>
-    <row r="11" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B11"/>
       <c r="E11"/>
       <c r="F11"/>
@@ -2702,7 +2943,7 @@
       <c r="J11"/>
       <c r="K11"/>
     </row>
-    <row r="12" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B12"/>
       <c r="E12"/>
       <c r="F12"/>
@@ -2710,7 +2951,7 @@
       <c r="J12"/>
       <c r="K12"/>
     </row>
-    <row r="13" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B13"/>
       <c r="E13"/>
       <c r="F13"/>
@@ -2718,7 +2959,7 @@
       <c r="J13"/>
       <c r="K13"/>
     </row>
-    <row r="14" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B14"/>
       <c r="E14"/>
       <c r="F14"/>
@@ -2726,7 +2967,7 @@
       <c r="J14"/>
       <c r="K14"/>
     </row>
-    <row r="15" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B15"/>
       <c r="E15"/>
       <c r="F15"/>
@@ -2734,7 +2975,7 @@
       <c r="J15"/>
       <c r="K15"/>
     </row>
-    <row r="16" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B16"/>
       <c r="E16"/>
       <c r="F16"/>
@@ -2742,7 +2983,7 @@
       <c r="J16"/>
       <c r="K16"/>
     </row>
-    <row r="17" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B17"/>
       <c r="E17"/>
       <c r="F17"/>
@@ -2750,7 +2991,7 @@
       <c r="J17"/>
       <c r="K17"/>
     </row>
-    <row r="18" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B18"/>
       <c r="E18"/>
       <c r="F18"/>
@@ -2758,7 +2999,7 @@
       <c r="J18"/>
       <c r="K18"/>
     </row>
-    <row r="19" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B19"/>
       <c r="E19"/>
       <c r="F19"/>
@@ -2766,7 +3007,7 @@
       <c r="J19"/>
       <c r="K19"/>
     </row>
-    <row r="20" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B20"/>
       <c r="E20"/>
       <c r="F20"/>
@@ -2774,7 +3015,7 @@
       <c r="J20"/>
       <c r="K20"/>
     </row>
-    <row r="21" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B21"/>
       <c r="E21"/>
       <c r="F21"/>
@@ -2782,7 +3023,7 @@
       <c r="J21"/>
       <c r="K21"/>
     </row>
-    <row r="22" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B22"/>
       <c r="E22"/>
       <c r="F22"/>
@@ -2790,7 +3031,7 @@
       <c r="J22"/>
       <c r="K22"/>
     </row>
-    <row r="23" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B23"/>
       <c r="E23"/>
       <c r="F23"/>
@@ -2798,7 +3039,7 @@
       <c r="J23"/>
       <c r="K23"/>
     </row>
-    <row r="24" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B24"/>
       <c r="E24"/>
       <c r="F24"/>
@@ -2806,7 +3047,7 @@
       <c r="J24"/>
       <c r="K24"/>
     </row>
-    <row r="25" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B25"/>
       <c r="E25"/>
       <c r="F25"/>
@@ -2814,7 +3055,7 @@
       <c r="J25"/>
       <c r="K25"/>
     </row>
-    <row r="26" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B26"/>
       <c r="E26"/>
       <c r="F26"/>
@@ -2822,7 +3063,7 @@
       <c r="J26"/>
       <c r="K26"/>
     </row>
-    <row r="27" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B27"/>
       <c r="E27"/>
       <c r="F27"/>
@@ -2830,7 +3071,7 @@
       <c r="J27"/>
       <c r="K27"/>
     </row>
-    <row r="28" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B28"/>
       <c r="E28"/>
       <c r="F28"/>
@@ -2838,7 +3079,7 @@
       <c r="J28"/>
       <c r="K28"/>
     </row>
-    <row r="29" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B29"/>
       <c r="E29"/>
       <c r="F29"/>
@@ -2846,7 +3087,7 @@
       <c r="J29"/>
       <c r="K29"/>
     </row>
-    <row r="30" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B30"/>
       <c r="E30"/>
       <c r="F30"/>
@@ -2854,7 +3095,7 @@
       <c r="J30"/>
       <c r="K30"/>
     </row>
-    <row r="31" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B31"/>
       <c r="E31"/>
       <c r="F31"/>
@@ -2862,7 +3103,7 @@
       <c r="J31"/>
       <c r="K31"/>
     </row>
-    <row r="32" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B32"/>
       <c r="E32"/>
       <c r="F32"/>
@@ -2870,7 +3111,7 @@
       <c r="J32"/>
       <c r="K32"/>
     </row>
-    <row r="33" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B33"/>
       <c r="E33"/>
       <c r="F33"/>
@@ -2878,7 +3119,7 @@
       <c r="J33"/>
       <c r="K33"/>
     </row>
-    <row r="34" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B34"/>
       <c r="E34"/>
       <c r="F34"/>
@@ -2886,7 +3127,7 @@
       <c r="J34"/>
       <c r="K34"/>
     </row>
-    <row r="35" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B35"/>
       <c r="E35"/>
       <c r="F35"/>
@@ -2894,7 +3135,7 @@
       <c r="J35"/>
       <c r="K35"/>
     </row>
-    <row r="36" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B36"/>
       <c r="E36"/>
       <c r="F36"/>
@@ -2902,7 +3143,7 @@
       <c r="J36"/>
       <c r="K36"/>
     </row>
-    <row r="37" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B37"/>
       <c r="E37"/>
       <c r="F37"/>
@@ -2910,7 +3151,7 @@
       <c r="J37"/>
       <c r="K37"/>
     </row>
-    <row r="38" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B38"/>
       <c r="E38"/>
       <c r="F38"/>
@@ -2918,7 +3159,7 @@
       <c r="J38"/>
       <c r="K38"/>
     </row>
-    <row r="39" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B39"/>
       <c r="E39"/>
       <c r="F39"/>
@@ -2926,7 +3167,7 @@
       <c r="J39"/>
       <c r="K39"/>
     </row>
-    <row r="40" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B40"/>
       <c r="E40"/>
       <c r="F40"/>
@@ -2934,7 +3175,7 @@
       <c r="J40"/>
       <c r="K40"/>
     </row>
-    <row r="41" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B41"/>
       <c r="E41"/>
       <c r="F41"/>
@@ -2942,7 +3183,7 @@
       <c r="J41"/>
       <c r="K41"/>
     </row>
-    <row r="42" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B42"/>
       <c r="E42"/>
       <c r="F42"/>
@@ -2950,7 +3191,7 @@
       <c r="J42"/>
       <c r="K42"/>
     </row>
-    <row r="43" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B43"/>
       <c r="E43"/>
       <c r="F43"/>
@@ -2958,7 +3199,7 @@
       <c r="J43"/>
       <c r="K43"/>
     </row>
-    <row r="44" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B44"/>
       <c r="E44"/>
       <c r="F44"/>
@@ -2966,7 +3207,7 @@
       <c r="J44"/>
       <c r="K44"/>
     </row>
-    <row r="45" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B45"/>
       <c r="E45"/>
       <c r="F45"/>
@@ -2974,7 +3215,7 @@
       <c r="J45"/>
       <c r="K45"/>
     </row>
-    <row r="46" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B46"/>
       <c r="E46"/>
       <c r="F46"/>
@@ -2982,7 +3223,7 @@
       <c r="J46"/>
       <c r="K46"/>
     </row>
-    <row r="47" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B47"/>
       <c r="E47"/>
       <c r="F47"/>
@@ -2990,7 +3231,7 @@
       <c r="J47"/>
       <c r="K47"/>
     </row>
-    <row r="48" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B48"/>
       <c r="E48"/>
       <c r="F48"/>
@@ -2998,7 +3239,7 @@
       <c r="J48"/>
       <c r="K48"/>
     </row>
-    <row r="49" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B49"/>
       <c r="E49"/>
       <c r="F49"/>
@@ -3006,7 +3247,7 @@
       <c r="J49"/>
       <c r="K49"/>
     </row>
-    <row r="50" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B50"/>
       <c r="E50"/>
       <c r="F50"/>
@@ -3014,7 +3255,7 @@
       <c r="J50"/>
       <c r="K50"/>
     </row>
-    <row r="51" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B51"/>
       <c r="E51"/>
       <c r="F51"/>
@@ -3022,7 +3263,7 @@
       <c r="J51"/>
       <c r="K51"/>
     </row>
-    <row r="52" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B52"/>
       <c r="E52"/>
       <c r="F52"/>
@@ -3030,7 +3271,7 @@
       <c r="J52"/>
       <c r="K52"/>
     </row>
-    <row r="53" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B53"/>
       <c r="E53"/>
       <c r="F53"/>
@@ -3038,7 +3279,7 @@
       <c r="J53"/>
       <c r="K53"/>
     </row>
-    <row r="54" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B54"/>
       <c r="E54"/>
       <c r="F54"/>
@@ -3046,7 +3287,7 @@
       <c r="J54"/>
       <c r="K54"/>
     </row>
-    <row r="55" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B55"/>
       <c r="E55"/>
       <c r="F55"/>
@@ -3054,7 +3295,7 @@
       <c r="J55"/>
       <c r="K55"/>
     </row>
-    <row r="56" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B56"/>
       <c r="E56"/>
       <c r="F56"/>
@@ -3062,7 +3303,7 @@
       <c r="J56"/>
       <c r="K56"/>
     </row>
-    <row r="57" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B57"/>
       <c r="E57"/>
       <c r="F57"/>
@@ -3070,7 +3311,7 @@
       <c r="J57"/>
       <c r="K57"/>
     </row>
-    <row r="58" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B58"/>
       <c r="E58"/>
       <c r="F58"/>
@@ -3078,7 +3319,7 @@
       <c r="J58"/>
       <c r="K58"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" s="30"/>
       <c r="B59"/>
       <c r="C59" s="30"/>
@@ -3090,7 +3331,7 @@
       <c r="J59"/>
       <c r="K59"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" s="30"/>
       <c r="B60"/>
       <c r="C60" s="30"/>
@@ -3102,7 +3343,7 @@
       <c r="J60"/>
       <c r="K60"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" s="30"/>
       <c r="B61"/>
       <c r="C61" s="30"/>
@@ -3114,7 +3355,7 @@
       <c r="J61"/>
       <c r="K61"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" s="30"/>
       <c r="B62"/>
       <c r="C62" s="30"/>
@@ -3126,7 +3367,7 @@
       <c r="J62"/>
       <c r="K62"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" s="30"/>
       <c r="B63"/>
       <c r="C63" s="30"/>
@@ -3138,7 +3379,7 @@
       <c r="J63"/>
       <c r="K63"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" s="30"/>
       <c r="B64"/>
       <c r="C64" s="30"/>
@@ -3150,7 +3391,7 @@
       <c r="J64"/>
       <c r="K64"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" s="30"/>
       <c r="B65"/>
       <c r="C65" s="30"/>
@@ -3162,7 +3403,7 @@
       <c r="J65"/>
       <c r="K65"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" s="30"/>
       <c r="B66"/>
       <c r="C66" s="30"/>
@@ -3174,7 +3415,7 @@
       <c r="J66"/>
       <c r="K66"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" s="30"/>
       <c r="B67"/>
       <c r="C67" s="30"/>
@@ -3186,7 +3427,7 @@
       <c r="J67"/>
       <c r="K67"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" s="30"/>
       <c r="B68"/>
       <c r="C68" s="30"/>
@@ -3198,7 +3439,7 @@
       <c r="J68"/>
       <c r="K68"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" s="30"/>
       <c r="B69"/>
       <c r="C69" s="30"/>
@@ -3210,7 +3451,7 @@
       <c r="J69"/>
       <c r="K69"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" s="30"/>
       <c r="B70"/>
       <c r="C70" s="30"/>
@@ -3222,7 +3463,7 @@
       <c r="J70"/>
       <c r="K70"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" s="30"/>
       <c r="B71"/>
       <c r="C71" s="30"/>
@@ -3234,7 +3475,7 @@
       <c r="J71"/>
       <c r="K71"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" s="30"/>
       <c r="B72"/>
       <c r="C72" s="30"/>
@@ -3246,7 +3487,7 @@
       <c r="J72"/>
       <c r="K72"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" s="30"/>
       <c r="B73"/>
       <c r="C73" s="30"/>
@@ -3258,7 +3499,7 @@
       <c r="J73"/>
       <c r="K73"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" s="30"/>
       <c r="B74"/>
       <c r="C74" s="30"/>
@@ -3270,7 +3511,7 @@
       <c r="J74"/>
       <c r="K74"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" s="30"/>
       <c r="B75"/>
       <c r="C75" s="30"/>
@@ -3282,7 +3523,7 @@
       <c r="J75"/>
       <c r="K75"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" s="30"/>
       <c r="B76"/>
       <c r="C76" s="30"/>
@@ -3294,7 +3535,7 @@
       <c r="J76"/>
       <c r="K76"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" s="30"/>
       <c r="B77"/>
       <c r="C77" s="30"/>
@@ -3306,7 +3547,7 @@
       <c r="J77"/>
       <c r="K77"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" s="30"/>
       <c r="B78"/>
       <c r="C78" s="30"/>
@@ -3318,7 +3559,7 @@
       <c r="J78"/>
       <c r="K78"/>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" s="30"/>
       <c r="B79"/>
       <c r="C79" s="30"/>
@@ -3330,7 +3571,7 @@
       <c r="J79"/>
       <c r="K79"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" s="30"/>
       <c r="B80"/>
       <c r="C80" s="30"/>
@@ -3342,7 +3583,7 @@
       <c r="J80"/>
       <c r="K80"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81" s="30"/>
       <c r="B81"/>
       <c r="C81" s="30"/>
@@ -3354,7 +3595,7 @@
       <c r="J81"/>
       <c r="K81"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82" s="30"/>
       <c r="B82"/>
       <c r="C82" s="30"/>
@@ -3366,7 +3607,7 @@
       <c r="J82"/>
       <c r="K82"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83" s="30"/>
       <c r="B83"/>
       <c r="C83" s="30"/>
@@ -3378,7 +3619,7 @@
       <c r="J83"/>
       <c r="K83"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84" s="30"/>
       <c r="B84"/>
       <c r="C84" s="30"/>
@@ -3390,7 +3631,7 @@
       <c r="J84"/>
       <c r="K84"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85" s="30"/>
       <c r="B85"/>
       <c r="C85" s="30"/>
@@ -3402,7 +3643,7 @@
       <c r="J85"/>
       <c r="K85"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86" s="30"/>
       <c r="B86"/>
       <c r="C86" s="30"/>
@@ -3414,7 +3655,7 @@
       <c r="J86"/>
       <c r="K86"/>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87" s="30"/>
       <c r="B87"/>
       <c r="C87" s="30"/>
@@ -3426,7 +3667,7 @@
       <c r="J87"/>
       <c r="K87"/>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A88" s="30"/>
       <c r="B88"/>
       <c r="C88" s="30"/>
@@ -3438,7 +3679,7 @@
       <c r="J88"/>
       <c r="K88"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89" s="30"/>
       <c r="B89"/>
       <c r="C89" s="30"/>
@@ -3450,7 +3691,7 @@
       <c r="J89"/>
       <c r="K89"/>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A90" s="30"/>
       <c r="B90"/>
       <c r="C90" s="30"/>
@@ -3462,7 +3703,7 @@
       <c r="J90"/>
       <c r="K90"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91" s="30"/>
       <c r="B91"/>
       <c r="C91" s="30"/>
@@ -3492,17 +3733,17 @@
       <selection activeCell="E29" sqref="A2:E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="6" width="8.7109375" style="1"/>
-    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" style="1"/>
-    <col min="10" max="10" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="6" width="8.6640625" style="1"/>
+    <col min="7" max="7" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="8.6640625" style="1"/>
+    <col min="10" max="10" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>23</v>
       </c>
@@ -3543,7 +3784,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2"/>
       <c r="C2"/>
@@ -3557,7 +3798,7 @@
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B3"/>
       <c r="C3"/>
       <c r="D3"/>
@@ -3567,7 +3808,7 @@
       <c r="H3"/>
       <c r="J3" s="42"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B4"/>
       <c r="C4"/>
       <c r="D4"/>
@@ -3577,7 +3818,7 @@
       <c r="H4"/>
       <c r="J4" s="42"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B5"/>
       <c r="C5"/>
       <c r="D5"/>
@@ -3588,7 +3829,7 @@
       <c r="I5" s="2"/>
       <c r="J5" s="42"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B6"/>
       <c r="C6"/>
       <c r="D6"/>
@@ -3599,7 +3840,7 @@
       <c r="I6" s="2"/>
       <c r="J6" s="42"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B7"/>
       <c r="C7"/>
       <c r="D7"/>
@@ -3610,7 +3851,7 @@
       <c r="I7" s="2"/>
       <c r="J7" s="42"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B8"/>
       <c r="C8"/>
       <c r="D8"/>
@@ -3621,7 +3862,7 @@
       <c r="I8" s="2"/>
       <c r="J8" s="42"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B9"/>
       <c r="C9"/>
       <c r="D9"/>
@@ -3632,7 +3873,7 @@
       <c r="I9" s="2"/>
       <c r="J9" s="42"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B10"/>
       <c r="C10"/>
       <c r="D10"/>
@@ -3643,7 +3884,7 @@
       <c r="I10" s="2"/>
       <c r="J10" s="42"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B11"/>
       <c r="C11"/>
       <c r="D11"/>
@@ -3654,7 +3895,7 @@
       <c r="I11" s="2"/>
       <c r="J11" s="42"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B12"/>
       <c r="C12"/>
       <c r="D12"/>
@@ -3665,7 +3906,7 @@
       <c r="I12" s="2"/>
       <c r="J12" s="42"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B13"/>
       <c r="C13"/>
       <c r="D13"/>
@@ -3676,7 +3917,7 @@
       <c r="I13" s="2"/>
       <c r="J13" s="42"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B14"/>
       <c r="C14"/>
       <c r="D14"/>
@@ -3687,7 +3928,7 @@
       <c r="I14" s="2"/>
       <c r="J14" s="42"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B15"/>
       <c r="C15"/>
       <c r="D15"/>
@@ -3698,7 +3939,7 @@
       <c r="I15" s="2"/>
       <c r="J15" s="42"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B16"/>
       <c r="C16"/>
       <c r="D16"/>
@@ -3709,7 +3950,7 @@
       <c r="I16" s="2"/>
       <c r="J16" s="42"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B17"/>
       <c r="C17"/>
       <c r="D17"/>
@@ -3719,7 +3960,7 @@
       <c r="H17"/>
       <c r="J17" s="42"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B18"/>
       <c r="C18"/>
       <c r="D18"/>
@@ -3729,7 +3970,7 @@
       <c r="H18"/>
       <c r="J18" s="42"/>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B19"/>
       <c r="C19"/>
       <c r="D19"/>
@@ -3739,7 +3980,7 @@
       <c r="H19"/>
       <c r="J19" s="42"/>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B20"/>
       <c r="C20"/>
       <c r="D20"/>
@@ -3749,7 +3990,7 @@
       <c r="H20"/>
       <c r="J20" s="42"/>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B21"/>
       <c r="C21"/>
       <c r="D21"/>
@@ -3759,7 +4000,7 @@
       <c r="H21"/>
       <c r="J21" s="42"/>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B22"/>
       <c r="C22"/>
       <c r="D22"/>
@@ -3769,7 +4010,7 @@
       <c r="H22"/>
       <c r="J22" s="42"/>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B23"/>
       <c r="C23"/>
       <c r="D23"/>
@@ -3779,7 +4020,7 @@
       <c r="H23"/>
       <c r="J23" s="42"/>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B24"/>
       <c r="C24"/>
       <c r="D24"/>
@@ -3789,7 +4030,7 @@
       <c r="H24"/>
       <c r="J24" s="42"/>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B25"/>
       <c r="C25"/>
       <c r="D25"/>
@@ -3799,7 +4040,7 @@
       <c r="H25"/>
       <c r="J25" s="42"/>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B26"/>
       <c r="C26"/>
       <c r="D26"/>
@@ -3809,7 +4050,7 @@
       <c r="H26"/>
       <c r="J26" s="42"/>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B27"/>
       <c r="C27"/>
       <c r="D27"/>
@@ -3819,7 +4060,7 @@
       <c r="H27"/>
       <c r="J27" s="42"/>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B28"/>
       <c r="C28"/>
       <c r="D28"/>
@@ -3829,7 +4070,7 @@
       <c r="H28"/>
       <c r="J28" s="42"/>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B29"/>
       <c r="C29"/>
       <c r="D29"/>
@@ -3852,16 +4093,16 @@
       <selection activeCell="A2" sqref="A2:XFD33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="11" width="8.7109375" style="5" customWidth="1"/>
-    <col min="12" max="28" width="8.7109375" style="1" customWidth="1"/>
-    <col min="29" max="29" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="63" width="8.7109375" style="1" customWidth="1"/>
-    <col min="64" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="11" width="8.6640625" style="5" customWidth="1"/>
+    <col min="12" max="28" width="8.6640625" style="1" customWidth="1"/>
+    <col min="29" max="29" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="63" width="8.6640625" style="1" customWidth="1"/>
+    <col min="64" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:59" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>23</v>
       </c>
@@ -3970,7 +4211,7 @@
       <c r="AR1" s="27"/>
       <c r="AS1" s="28"/>
     </row>
-    <row r="2" spans="1:59" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:59" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="30"/>
       <c r="B2"/>
       <c r="C2"/>
@@ -4011,7 +4252,7 @@
       <c r="AR2" s="30"/>
       <c r="AS2" s="30"/>
     </row>
-    <row r="3" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A3" s="30"/>
       <c r="B3"/>
       <c r="C3"/>
@@ -4044,7 +4285,7 @@
       <c r="AD3" s="30"/>
       <c r="AE3" s="30"/>
     </row>
-    <row r="4" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A4" s="30"/>
       <c r="B4"/>
       <c r="C4"/>
@@ -4077,7 +4318,7 @@
       <c r="AD4" s="30"/>
       <c r="AE4" s="30"/>
     </row>
-    <row r="5" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A5" s="30"/>
       <c r="B5"/>
       <c r="C5"/>
@@ -4138,7 +4379,7 @@
       <c r="BF5" s="17"/>
       <c r="BG5" s="17"/>
     </row>
-    <row r="6" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A6" s="30"/>
       <c r="B6"/>
       <c r="C6"/>
@@ -4166,7 +4407,7 @@
       <c r="AD6" s="30"/>
       <c r="AE6" s="30"/>
     </row>
-    <row r="7" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A7" s="30"/>
       <c r="B7"/>
       <c r="C7"/>
@@ -4194,7 +4435,7 @@
       <c r="AD7" s="30"/>
       <c r="AE7" s="30"/>
     </row>
-    <row r="8" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A8" s="30"/>
       <c r="B8"/>
       <c r="C8"/>
@@ -4222,7 +4463,7 @@
       <c r="AD8" s="30"/>
       <c r="AE8" s="30"/>
     </row>
-    <row r="9" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A9" s="30"/>
       <c r="B9"/>
       <c r="C9"/>
@@ -4250,7 +4491,7 @@
       <c r="AD9" s="30"/>
       <c r="AE9" s="30"/>
     </row>
-    <row r="10" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A10" s="30"/>
       <c r="B10"/>
       <c r="C10"/>
@@ -4278,7 +4519,7 @@
       <c r="AD10" s="30"/>
       <c r="AE10" s="30"/>
     </row>
-    <row r="11" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A11" s="30"/>
       <c r="B11"/>
       <c r="C11"/>
@@ -4306,7 +4547,7 @@
       <c r="AD11" s="30"/>
       <c r="AE11" s="30"/>
     </row>
-    <row r="12" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A12" s="30"/>
       <c r="B12"/>
       <c r="C12"/>
@@ -4334,7 +4575,7 @@
       <c r="AD12" s="30"/>
       <c r="AE12" s="30"/>
     </row>
-    <row r="13" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A13" s="30"/>
       <c r="B13"/>
       <c r="C13"/>
@@ -4362,7 +4603,7 @@
       <c r="AD13" s="30"/>
       <c r="AE13" s="30"/>
     </row>
-    <row r="14" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A14" s="30"/>
       <c r="B14"/>
       <c r="C14"/>
@@ -4390,7 +4631,7 @@
       <c r="AD14" s="30"/>
       <c r="AE14" s="30"/>
     </row>
-    <row r="15" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A15" s="30"/>
       <c r="B15"/>
       <c r="C15"/>
@@ -4418,7 +4659,7 @@
       <c r="AD15" s="30"/>
       <c r="AE15" s="30"/>
     </row>
-    <row r="16" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A16" s="30"/>
       <c r="B16"/>
       <c r="C16"/>
@@ -4446,7 +4687,7 @@
       <c r="AD16" s="30"/>
       <c r="AE16" s="30"/>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A17" s="30"/>
       <c r="B17"/>
       <c r="C17"/>
@@ -4474,7 +4715,7 @@
       <c r="AD17" s="30"/>
       <c r="AE17" s="30"/>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A18" s="30"/>
       <c r="B18"/>
       <c r="C18"/>
@@ -4502,7 +4743,7 @@
       <c r="AD18" s="30"/>
       <c r="AE18" s="30"/>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A19" s="30"/>
       <c r="B19"/>
       <c r="C19"/>
@@ -4530,7 +4771,7 @@
       <c r="AD19" s="30"/>
       <c r="AE19" s="30"/>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A20" s="30"/>
       <c r="B20"/>
       <c r="C20"/>
@@ -4558,7 +4799,7 @@
       <c r="AD20" s="30"/>
       <c r="AE20" s="30"/>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A21" s="30"/>
       <c r="B21"/>
       <c r="C21"/>
@@ -4586,7 +4827,7 @@
       <c r="AD21" s="30"/>
       <c r="AE21" s="30"/>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A22" s="30"/>
       <c r="B22"/>
       <c r="C22"/>
@@ -4614,7 +4855,7 @@
       <c r="AD22" s="30"/>
       <c r="AE22" s="30"/>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A23" s="30"/>
       <c r="B23"/>
       <c r="C23"/>
@@ -4642,7 +4883,7 @@
       <c r="AD23" s="30"/>
       <c r="AE23" s="30"/>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A24" s="30"/>
       <c r="B24"/>
       <c r="C24"/>
@@ -4670,7 +4911,7 @@
       <c r="AD24" s="30"/>
       <c r="AE24" s="30"/>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A25" s="30"/>
       <c r="B25"/>
       <c r="C25"/>
@@ -4698,7 +4939,7 @@
       <c r="AD25" s="30"/>
       <c r="AE25" s="30"/>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A26" s="30"/>
       <c r="B26"/>
       <c r="C26"/>
@@ -4726,7 +4967,7 @@
       <c r="AD26" s="30"/>
       <c r="AE26" s="30"/>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A27" s="30"/>
       <c r="B27"/>
       <c r="C27"/>
@@ -4754,7 +4995,7 @@
       <c r="AD27" s="30"/>
       <c r="AE27" s="30"/>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A28" s="30"/>
       <c r="B28"/>
       <c r="C28"/>
@@ -4782,7 +5023,7 @@
       <c r="AD28" s="30"/>
       <c r="AE28" s="30"/>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A29" s="30"/>
       <c r="B29"/>
       <c r="C29"/>
@@ -4839,12 +5080,12 @@
       <selection activeCell="A2" sqref="A2:XFD268"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="8.7109375" style="2"/>
+    <col min="1" max="16384" width="8.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="39" t="s">
         <v>23</v>
       </c>
@@ -4882,7 +5123,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="30"/>
       <c r="B2"/>
       <c r="C2"/>
@@ -4892,7 +5133,7 @@
       <c r="G2"/>
       <c r="H2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="30"/>
       <c r="B3"/>
       <c r="C3"/>
@@ -4902,7 +5143,7 @@
       <c r="G3"/>
       <c r="H3"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="30"/>
       <c r="B4"/>
       <c r="C4"/>
@@ -4912,7 +5153,7 @@
       <c r="G4"/>
       <c r="H4"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="30"/>
       <c r="B5"/>
       <c r="C5"/>
@@ -4922,7 +5163,7 @@
       <c r="G5"/>
       <c r="H5"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="30"/>
       <c r="B6"/>
       <c r="C6"/>
@@ -4932,7 +5173,7 @@
       <c r="G6"/>
       <c r="H6"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="30"/>
       <c r="B7"/>
       <c r="C7"/>
@@ -4942,7 +5183,7 @@
       <c r="G7"/>
       <c r="H7"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="30"/>
       <c r="B8"/>
       <c r="C8"/>
@@ -4952,7 +5193,7 @@
       <c r="G8"/>
       <c r="H8"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="30"/>
       <c r="B9"/>
       <c r="C9"/>
@@ -4962,7 +5203,7 @@
       <c r="G9"/>
       <c r="H9"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="30"/>
       <c r="B10"/>
       <c r="C10"/>
@@ -4972,7 +5213,7 @@
       <c r="G10"/>
       <c r="H10"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="30"/>
       <c r="B11"/>
       <c r="C11"/>
@@ -4982,7 +5223,7 @@
       <c r="G11"/>
       <c r="H11"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="30"/>
       <c r="B12"/>
       <c r="C12"/>
@@ -4992,7 +5233,7 @@
       <c r="G12"/>
       <c r="H12"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="30"/>
       <c r="B13"/>
       <c r="C13"/>
@@ -5002,7 +5243,7 @@
       <c r="G13"/>
       <c r="H13"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="30"/>
       <c r="B14"/>
       <c r="C14"/>
@@ -5012,7 +5253,7 @@
       <c r="G14"/>
       <c r="H14"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="30"/>
       <c r="B15"/>
       <c r="C15"/>
@@ -5022,7 +5263,7 @@
       <c r="G15"/>
       <c r="H15"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="30"/>
       <c r="B16"/>
       <c r="C16"/>
@@ -5032,7 +5273,7 @@
       <c r="G16"/>
       <c r="H16"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="30"/>
       <c r="B17"/>
       <c r="C17"/>
@@ -5042,7 +5283,7 @@
       <c r="G17"/>
       <c r="H17"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="30"/>
       <c r="B18"/>
       <c r="C18"/>
@@ -5052,7 +5293,7 @@
       <c r="G18"/>
       <c r="H18"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="30"/>
       <c r="B19"/>
       <c r="C19"/>
@@ -5062,7 +5303,7 @@
       <c r="G19"/>
       <c r="H19"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="30"/>
       <c r="B20"/>
       <c r="C20"/>
@@ -5072,7 +5313,7 @@
       <c r="G20"/>
       <c r="H20"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="30"/>
       <c r="B21"/>
       <c r="C21"/>
@@ -5082,7 +5323,7 @@
       <c r="G21"/>
       <c r="H21"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="30"/>
       <c r="B22"/>
       <c r="C22"/>
@@ -5092,7 +5333,7 @@
       <c r="G22"/>
       <c r="H22"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="30"/>
       <c r="B23"/>
       <c r="C23"/>
@@ -5102,7 +5343,7 @@
       <c r="G23"/>
       <c r="H23"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="30"/>
       <c r="B24"/>
       <c r="C24"/>
@@ -5112,7 +5353,7 @@
       <c r="G24"/>
       <c r="H24"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="30"/>
       <c r="B25"/>
       <c r="C25"/>
@@ -5122,7 +5363,7 @@
       <c r="G25"/>
       <c r="H25"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="30"/>
       <c r="B26"/>
       <c r="C26"/>
@@ -5132,7 +5373,7 @@
       <c r="G26"/>
       <c r="H26"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="30"/>
       <c r="B27"/>
       <c r="C27"/>
@@ -5142,7 +5383,7 @@
       <c r="G27"/>
       <c r="H27"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="30"/>
       <c r="B28"/>
       <c r="C28"/>
@@ -5152,7 +5393,7 @@
       <c r="G28"/>
       <c r="H28"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="30"/>
       <c r="B29"/>
       <c r="C29"/>
@@ -5162,7 +5403,7 @@
       <c r="G29"/>
       <c r="H29"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="30"/>
       <c r="B30"/>
       <c r="C30"/>
@@ -5172,7 +5413,7 @@
       <c r="G30"/>
       <c r="H30"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="30"/>
       <c r="B31"/>
       <c r="C31"/>
@@ -5182,7 +5423,7 @@
       <c r="G31"/>
       <c r="H31"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="30"/>
       <c r="B32"/>
       <c r="C32"/>
@@ -5192,7 +5433,7 @@
       <c r="G32"/>
       <c r="H32"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="30"/>
       <c r="B33"/>
       <c r="C33"/>
@@ -5202,7 +5443,7 @@
       <c r="G33"/>
       <c r="H33"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="30"/>
       <c r="B34"/>
       <c r="C34"/>
@@ -5212,7 +5453,7 @@
       <c r="G34"/>
       <c r="H34"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="30"/>
       <c r="B35"/>
       <c r="C35"/>
@@ -5222,7 +5463,7 @@
       <c r="G35"/>
       <c r="H35"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="30"/>
       <c r="B36"/>
       <c r="C36"/>
@@ -5232,7 +5473,7 @@
       <c r="G36"/>
       <c r="H36"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="30"/>
       <c r="B37"/>
       <c r="C37"/>
@@ -5242,7 +5483,7 @@
       <c r="G37"/>
       <c r="H37"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="30"/>
       <c r="B38"/>
       <c r="C38"/>
@@ -5252,7 +5493,7 @@
       <c r="G38"/>
       <c r="H38"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="30"/>
       <c r="B39"/>
       <c r="C39"/>
@@ -5262,7 +5503,7 @@
       <c r="G39"/>
       <c r="H39"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="30"/>
       <c r="B40"/>
       <c r="C40"/>
@@ -5272,7 +5513,7 @@
       <c r="G40"/>
       <c r="H40"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="30"/>
       <c r="B41"/>
       <c r="C41"/>
@@ -5282,7 +5523,7 @@
       <c r="G41"/>
       <c r="H41"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="30"/>
       <c r="B42"/>
       <c r="C42"/>
@@ -5292,7 +5533,7 @@
       <c r="G42"/>
       <c r="H42"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="30"/>
       <c r="B43"/>
       <c r="C43"/>
@@ -5302,7 +5543,7 @@
       <c r="G43"/>
       <c r="H43"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="30"/>
       <c r="B44"/>
       <c r="C44"/>
@@ -5312,7 +5553,7 @@
       <c r="G44"/>
       <c r="H44"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="30"/>
       <c r="B45"/>
       <c r="C45"/>
@@ -5322,7 +5563,7 @@
       <c r="G45"/>
       <c r="H45"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="30"/>
       <c r="B46"/>
       <c r="C46"/>
@@ -5332,7 +5573,7 @@
       <c r="G46"/>
       <c r="H46"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="30"/>
       <c r="B47"/>
       <c r="C47"/>
@@ -5342,7 +5583,7 @@
       <c r="G47"/>
       <c r="H47"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="30"/>
       <c r="B48"/>
       <c r="C48"/>
@@ -5352,7 +5593,7 @@
       <c r="G48"/>
       <c r="H48"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="30"/>
       <c r="B49"/>
       <c r="C49"/>
@@ -5362,7 +5603,7 @@
       <c r="G49"/>
       <c r="H49"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" s="30"/>
       <c r="B50"/>
       <c r="C50"/>
@@ -5372,7 +5613,7 @@
       <c r="G50"/>
       <c r="H50"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="30"/>
       <c r="B51"/>
       <c r="C51"/>
@@ -5382,7 +5623,7 @@
       <c r="G51"/>
       <c r="H51"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="30"/>
       <c r="B52"/>
       <c r="C52"/>
@@ -5392,7 +5633,7 @@
       <c r="G52"/>
       <c r="H52"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" s="30"/>
       <c r="B53"/>
       <c r="C53"/>
@@ -5402,7 +5643,7 @@
       <c r="G53"/>
       <c r="H53"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="30"/>
       <c r="B54"/>
       <c r="C54"/>
@@ -5412,7 +5653,7 @@
       <c r="G54"/>
       <c r="H54"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="30"/>
       <c r="B55"/>
       <c r="C55"/>
@@ -5422,7 +5663,7 @@
       <c r="G55"/>
       <c r="H55"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="30"/>
       <c r="B56"/>
       <c r="C56"/>

</xml_diff>

<commit_message>
clear trafo and add shunt in headers files
</commit_message>
<xml_diff>
--- a/stability_analysis/data/cases/IEEE_118_FULL_headers.xlsx
+++ b/stability_analysis/data/cases/IEEE_118_FULL_headers.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Francesca\miniconda3\envs\gridcal_original\stability_analysis\stability_analysis\data\cases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Francesca\miniconda3\envs\hp2c-dt\stability_analysis\stability_analysis\data\cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0667D2FC-3759-42F8-BFC8-AB6EE5B53DEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A796860A-6CC6-4009-8C8E-29D5BCA7DC48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="922" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="922" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gen" sheetId="20" r:id="rId1"/>
@@ -4260,7 +4260,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17CFBF60-98A8-4115-AF57-8C42FECC4BBB}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
@@ -4505,8 +4505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E717AAA3-63C1-47BF-9E0D-1A781E3C2FDE}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4547,273 +4547,49 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="11">
-        <v>1</v>
-      </c>
-      <c r="B2" s="11">
-        <v>5</v>
-      </c>
-      <c r="C2" s="11">
-        <v>8</v>
-      </c>
-      <c r="D2" s="11">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>2.6700000000000002E-2</v>
-      </c>
-      <c r="F2" s="12">
-        <v>0</v>
-      </c>
-      <c r="G2" s="11">
-        <v>1</v>
-      </c>
-      <c r="H2" s="11">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
+      <c r="E2"/>
+      <c r="F2" s="12"/>
+      <c r="I2"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="11">
-        <f>A2+1</f>
-        <v>2</v>
-      </c>
-      <c r="B3" s="11">
-        <v>17</v>
-      </c>
-      <c r="C3" s="11">
-        <v>30</v>
-      </c>
-      <c r="D3" s="11">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>3.8800000000000001E-2</v>
-      </c>
-      <c r="F3" s="12">
-        <v>0</v>
-      </c>
-      <c r="G3" s="11">
-        <v>1</v>
-      </c>
-      <c r="H3" s="11">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
+      <c r="E3"/>
+      <c r="F3" s="12"/>
+      <c r="I3"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="11">
-        <f t="shared" ref="A4:A10" si="0">A3+1</f>
-        <v>3</v>
-      </c>
-      <c r="B4" s="11">
-        <v>25</v>
-      </c>
-      <c r="C4" s="11">
-        <v>26</v>
-      </c>
-      <c r="D4" s="11">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>3.8199999999999998E-2</v>
-      </c>
-      <c r="F4" s="12">
-        <v>0</v>
-      </c>
-      <c r="G4" s="11">
-        <v>1</v>
-      </c>
-      <c r="H4" s="11">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
+      <c r="E4"/>
+      <c r="F4" s="12"/>
+      <c r="I4"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="11">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B5" s="11">
-        <v>37</v>
-      </c>
-      <c r="C5" s="11">
-        <v>38</v>
-      </c>
-      <c r="D5" s="12">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>3.7499999999999999E-2</v>
-      </c>
-      <c r="F5" s="12">
-        <v>0</v>
-      </c>
-      <c r="G5" s="11">
-        <v>1</v>
-      </c>
-      <c r="H5" s="11">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
+      <c r="D5" s="12"/>
+      <c r="E5"/>
+      <c r="F5" s="12"/>
+      <c r="I5"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="11">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B6" s="11">
-        <v>59</v>
-      </c>
-      <c r="C6" s="11">
-        <v>63</v>
-      </c>
-      <c r="D6" s="12">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>3.8600000000000002E-2</v>
-      </c>
-      <c r="F6" s="12">
-        <v>0</v>
-      </c>
-      <c r="G6" s="11">
-        <v>1</v>
-      </c>
-      <c r="H6" s="11">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
+      <c r="D6" s="12"/>
+      <c r="E6"/>
+      <c r="F6" s="12"/>
+      <c r="I6"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="11">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B7" s="11">
-        <v>61</v>
-      </c>
-      <c r="C7" s="11">
-        <v>64</v>
-      </c>
-      <c r="D7" s="11">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>2.6800000000000001E-2</v>
-      </c>
-      <c r="F7" s="12">
-        <v>0</v>
-      </c>
-      <c r="G7" s="11">
-        <v>1</v>
-      </c>
-      <c r="H7" s="11">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
+      <c r="E7"/>
+      <c r="F7" s="12"/>
+      <c r="I7"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="11">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="B8" s="11">
-        <v>65</v>
-      </c>
-      <c r="C8" s="11">
-        <v>66</v>
-      </c>
-      <c r="D8" s="11">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>3.6999999999999998E-2</v>
-      </c>
-      <c r="F8" s="12">
-        <v>0</v>
-      </c>
-      <c r="G8" s="11">
-        <v>1</v>
-      </c>
-      <c r="H8" s="11">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
+      <c r="E8"/>
+      <c r="F8" s="12"/>
+      <c r="I8"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="11">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="B9" s="11">
-        <v>68</v>
-      </c>
-      <c r="C9" s="11">
-        <v>69</v>
-      </c>
-      <c r="D9" s="11">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>3.6999999999999998E-2</v>
-      </c>
-      <c r="F9" s="11">
-        <v>0</v>
-      </c>
-      <c r="G9" s="11">
-        <v>1</v>
-      </c>
-      <c r="H9" s="11">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
+      <c r="E9"/>
+      <c r="I9"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="11">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B10" s="11">
-        <v>80</v>
-      </c>
-      <c r="C10" s="11">
-        <v>81</v>
-      </c>
-      <c r="D10" s="11">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>3.6999999999999998E-2</v>
-      </c>
-      <c r="F10" s="11">
-        <v>0</v>
-      </c>
-      <c r="G10" s="11">
-        <v>1</v>
-      </c>
-      <c r="H10" s="11">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>1</v>
-      </c>
+      <c r="E10"/>
+      <c r="I10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>